<commit_message>
deleted stray calculation in old faithful data file
</commit_message>
<xml_diff>
--- a/Data/OldFaithful.xlsx
+++ b/Data/OldFaithful.xlsx
@@ -1,22 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rdcromar\Documents\FDMAT223\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://webmailbyui-my.sharepoint.com/personal/drp36_byui_edu/Documents/221/Course_Files/BYUI_M221_Book/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_C763C3F04D2340DF3BBD9EF82CDDAF4229BA55B5" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{6A87266D-004A-4271-9049-F604C5D4952D}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="30" windowWidth="8400" windowHeight="2400"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -53,7 +64,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -178,6 +189,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -213,6 +241,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -388,12 +433,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G273"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C273"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A273"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -3213,7 +3256,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="257" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A257">
         <v>3.8170000000000002</v>
       </c>
@@ -3224,7 +3267,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="258" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A258">
         <v>3.9169999999999998</v>
       </c>
@@ -3235,7 +3278,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="259" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A259">
         <v>4.45</v>
       </c>
@@ -3246,7 +3289,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="260" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A260">
         <v>2</v>
       </c>
@@ -3256,12 +3299,8 @@
       <c r="C260" t="s">
         <v>8</v>
       </c>
-      <c r="G260">
-        <f>(1.65-1.59)/0.026</f>
-        <v>2.3076923076923013</v>
-      </c>
-    </row>
-    <row r="261" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="261" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A261">
         <v>4.2830000000000004</v>
       </c>
@@ -3272,7 +3311,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="262" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A262">
         <v>4.7670000000000003</v>
       </c>
@@ -3283,7 +3322,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="263" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A263">
         <v>4.5330000000000004</v>
       </c>
@@ -3294,7 +3333,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="264" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A264">
         <v>1.85</v>
       </c>
@@ -3305,7 +3344,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="265" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A265">
         <v>4.25</v>
       </c>
@@ -3316,7 +3355,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="266" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A266">
         <v>1.9830000000000001</v>
       </c>
@@ -3327,7 +3366,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="267" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A267">
         <v>2.25</v>
       </c>
@@ -3338,7 +3377,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="268" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A268">
         <v>4.75</v>
       </c>
@@ -3349,7 +3388,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="269" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A269">
         <v>4.117</v>
       </c>
@@ -3360,7 +3399,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="270" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A270">
         <v>2.15</v>
       </c>
@@ -3371,7 +3410,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="271" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A271">
         <v>4.4169999999999998</v>
       </c>
@@ -3382,7 +3421,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="272" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A272">
         <v>1.8169999999999999</v>
       </c>
@@ -3411,7 +3450,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3423,7 +3462,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>